<commit_message>
Added new way to create purchase excel file(template)
</commit_message>
<xml_diff>
--- a/resources/website/static/purchase-template.xlsx
+++ b/resources/website/static/purchase-template.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ediapp\d$\inetpub\EDI_LIVE\Downloads\Book\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8800"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8796"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,9 +12,9 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -27,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="57">
   <si>
     <t>Nr.</t>
   </si>
@@ -195,13 +190,16 @@
   </si>
   <si>
     <t>Rregullimet për të ulur TVSH-në / Ngarkesa e kundërt për Energjinë me normë 8%</t>
+  </si>
+  <si>
+    <t>Totali</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -260,7 +258,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -393,21 +391,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top/>
       <bottom/>
@@ -464,6 +447,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -473,9 +471,7 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -488,9 +484,7 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -501,9 +495,7 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -516,9 +508,7 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -529,16 +519,27 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -552,7 +553,11 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
@@ -560,50 +565,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection hidden="1"/>
@@ -632,27 +605,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
@@ -665,6 +626,58 @@
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection hidden="1"/>
     </xf>
@@ -728,7 +741,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -763,7 +776,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -940,91 +953,91 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AC4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X6" sqref="X6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="4.36328125" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="3" max="3" width="17.6328125" customWidth="1"/>
-    <col min="4" max="4" width="27.6328125" customWidth="1"/>
-    <col min="5" max="5" width="13.54296875" customWidth="1"/>
-    <col min="6" max="6" width="11.453125" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" customWidth="1"/>
+    <col min="4" max="4" width="27.6640625" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" customWidth="1"/>
+    <col min="6" max="6" width="11.44140625" customWidth="1"/>
     <col min="7" max="10" width="13" customWidth="1"/>
-    <col min="11" max="11" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.6328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.08984375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.08984375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="9" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="10" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="11.6328125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="14.08984375" customWidth="1"/>
+    <col min="22" max="22" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:29" ht="15.6">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="30" t="s">
+      <c r="C1" s="21"/>
+      <c r="D1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="32"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="17" t="s">
+      <c r="E1" s="22"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="17" t="s">
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="18"/>
-      <c r="S1" s="19"/>
-      <c r="T1" s="20" t="s">
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="U1" s="21"/>
-      <c r="V1" s="21"/>
-      <c r="W1" s="21"/>
-      <c r="X1" s="21"/>
-      <c r="Y1" s="21"/>
-      <c r="Z1" s="21"/>
-      <c r="AA1" s="21"/>
-      <c r="AB1" s="22"/>
-      <c r="AC1" s="23" t="s">
+      <c r="U1" s="14"/>
+      <c r="V1" s="14"/>
+      <c r="W1" s="14"/>
+      <c r="X1" s="14"/>
+      <c r="Y1" s="14"/>
+      <c r="Z1" s="14"/>
+      <c r="AA1" s="14"/>
+      <c r="AB1" s="15"/>
+      <c r="AC1" s="16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="77" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="29"/>
+    <row r="2" spans="1:29" ht="76.95" customHeight="1" thickBot="1">
+      <c r="A2" s="19"/>
       <c r="B2" s="4" t="s">
         <v>7</v>
       </c>
@@ -1106,89 +1119,123 @@
       <c r="AB2" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="AC2" s="24"/>
+      <c r="AC2" s="17"/>
     </row>
-    <row r="3" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="25" t="s">
+    <row r="3" spans="1:29">
+      <c r="A3" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="10" t="s">
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="I3" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="K3" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="L3" s="11" t="s">
+      <c r="L3" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="M3" s="11" t="s">
+      <c r="M3" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="N3" s="11" t="s">
+      <c r="N3" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="O3" s="11" t="s">
+      <c r="O3" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="P3" s="11" t="s">
+      <c r="P3" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="Q3" s="11" t="s">
+      <c r="Q3" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="R3" s="11" t="s">
+      <c r="R3" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="S3" s="13" t="s">
+      <c r="S3" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="T3" s="14" t="s">
+      <c r="T3" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="U3" s="11" t="s">
+      <c r="U3" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="V3" s="11" t="s">
+      <c r="V3" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="W3" s="11" t="s">
+      <c r="W3" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="X3" s="11" t="s">
+      <c r="X3" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="Y3" s="11" t="s">
+      <c r="Y3" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="Z3" s="11" t="s">
+      <c r="Z3" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="AA3" s="11" t="s">
+      <c r="AA3" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="AB3" s="15" t="s">
+      <c r="AB3" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="AC3" s="16" t="s">
+      <c r="AC3" s="32" t="s">
         <v>49</v>
       </c>
+    </row>
+    <row r="4" spans="1:29">
+      <c r="A4" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="34"/>
+      <c r="K4" s="34"/>
+      <c r="L4" s="34"/>
+      <c r="M4" s="34"/>
+      <c r="N4" s="34"/>
+      <c r="O4" s="34"/>
+      <c r="P4" s="34"/>
+      <c r="Q4" s="34"/>
+      <c r="R4" s="34"/>
+      <c r="S4" s="35"/>
+      <c r="T4" s="34"/>
+      <c r="U4" s="34"/>
+      <c r="V4" s="34"/>
+      <c r="W4" s="34"/>
+      <c r="X4" s="34"/>
+      <c r="Y4" s="34"/>
+      <c r="Z4" s="34"/>
+      <c r="AA4" s="34"/>
+      <c r="AB4" s="35"/>
+      <c r="AC4" s="35"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
+    <mergeCell ref="A4:F4"/>
     <mergeCell ref="G1:J1"/>
     <mergeCell ref="K1:S1"/>
     <mergeCell ref="T1:AB1"/>

</xml_diff>